<commit_message>
common update 1 25.04.2022
</commit_message>
<xml_diff>
--- a/data/draft.xlsx
+++ b/data/draft.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20385"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ZLei\Documents\Git\tiSPHi\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Benutzer\Lei\Documents\Git\tiSPHi\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA3D8867-EF7C-46EE-A129-D696EB95C31E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53DC862-3D17-4A30-963C-E22F53A2A7D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" activeTab="2" xr2:uid="{F96AF2A0-9E31-4557-A308-4BAF8AA6954F}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="25815" windowHeight="15615" activeTab="2" xr2:uid="{F96AF2A0-9E31-4557-A308-4BAF8AA6954F}"/>
   </bookViews>
   <sheets>
     <sheet name="kernel" sheetId="1" r:id="rId1"/>
@@ -22,14 +22,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1958,7 +1950,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>-32.167603807643374</c:v>
+                  <c:v>-29</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1970,7 +1962,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2.5166114784235831</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3829,12 +3821,12 @@
       <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -3854,7 +3846,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -3878,7 +3870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D3" s="1">
         <v>-1.9</v>
       </c>
@@ -3895,7 +3887,7 @@
         <v>3.4104630662549059E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D4" s="1">
         <v>-1.8</v>
       </c>
@@ -3912,7 +3904,7 @@
         <v>1.3641852265019594E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D5" s="1">
         <v>-1.7</v>
       </c>
@@ -3929,7 +3921,7 @@
         <v>3.0694167596294109E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D6" s="1">
         <v>-1.6</v>
       </c>
@@ -3946,7 +3938,7 @@
         <v>5.4567409060078377E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D7" s="1">
         <v>-1.5</v>
       </c>
@@ -3963,7 +3955,7 @@
         <v>8.5261576656372504E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D8" s="1">
         <v>-1.4</v>
       </c>
@@ -3980,7 +3972,7 @@
         <v>0.12277667038517644</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D9" s="1">
         <v>-1.3</v>
       </c>
@@ -3997,7 +3989,7 @@
         <v>0.16711269024649009</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D10" s="1">
         <v>-1.2</v>
       </c>
@@ -4014,7 +4006,7 @@
         <v>0.21826963624031365</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D11" s="1">
         <v>-1.1000000000000001</v>
       </c>
@@ -4031,7 +4023,7 @@
         <v>0.27624750836664685</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D12" s="1">
         <v>-1</v>
       </c>
@@ -4048,7 +4040,7 @@
         <v>0.34104630662549001</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D13" s="1">
         <v>-0.9</v>
       </c>
@@ -4065,7 +4057,7 @@
         <v>0.39902417875182328</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D14" s="1">
         <v>-0.8</v>
       </c>
@@ -4082,7 +4074,7 @@
         <v>0.43653927248062713</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D15" s="1">
         <v>-0.7</v>
       </c>
@@ -4099,7 +4091,7 @@
         <v>0.45359158781190173</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D16" s="1">
         <v>-0.6</v>
       </c>
@@ -4116,7 +4108,7 @@
         <v>0.45018112474564675</v>
       </c>
     </row>
-    <row r="17" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D17" s="1">
         <v>-0.5</v>
       </c>
@@ -4133,7 +4125,7 @@
         <v>0.42630788328186253</v>
       </c>
     </row>
-    <row r="18" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D18" s="1">
         <v>-0.4</v>
       </c>
@@ -4150,7 +4142,7 @@
         <v>0.38197186342054884</v>
       </c>
     </row>
-    <row r="19" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D19" s="1">
         <v>-0.3</v>
       </c>
@@ -4167,7 +4159,7 @@
         <v>0.31717306516170568</v>
       </c>
     </row>
-    <row r="20" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D20" s="1">
         <v>-0.2</v>
       </c>
@@ -4184,7 +4176,7 @@
         <v>0.23191148850533322</v>
       </c>
     </row>
-    <row r="21" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D21" s="1">
         <v>-0.1</v>
       </c>
@@ -4201,7 +4193,7 @@
         <v>0.12618713345143132</v>
       </c>
     </row>
-    <row r="22" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D22" s="1">
         <v>0</v>
       </c>
@@ -4218,7 +4210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D23" s="1">
         <v>0.1</v>
       </c>
@@ -4235,7 +4227,7 @@
         <v>-0.12618713345143132</v>
       </c>
     </row>
-    <row r="24" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D24" s="1">
         <v>0.2</v>
       </c>
@@ -4252,7 +4244,7 @@
         <v>-0.23191148850533322</v>
       </c>
     </row>
-    <row r="25" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D25" s="1">
         <v>0.3</v>
       </c>
@@ -4269,7 +4261,7 @@
         <v>-0.31717306516170568</v>
       </c>
     </row>
-    <row r="26" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D26" s="1">
         <v>0.4</v>
       </c>
@@ -4286,7 +4278,7 @@
         <v>-0.38197186342054884</v>
       </c>
     </row>
-    <row r="27" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D27" s="1">
         <v>0.5</v>
       </c>
@@ -4303,7 +4295,7 @@
         <v>-0.42630788328186253</v>
       </c>
     </row>
-    <row r="28" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D28" s="1">
         <v>0.6</v>
       </c>
@@ -4320,7 +4312,7 @@
         <v>-0.45018112474564675</v>
       </c>
     </row>
-    <row r="29" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D29" s="1">
         <v>0.7</v>
       </c>
@@ -4337,7 +4329,7 @@
         <v>-0.45359158781190173</v>
       </c>
     </row>
-    <row r="30" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D30" s="1">
         <v>0.8</v>
       </c>
@@ -4354,7 +4346,7 @@
         <v>-0.43653927248062713</v>
       </c>
     </row>
-    <row r="31" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D31" s="1">
         <v>0.9</v>
       </c>
@@ -4371,7 +4363,7 @@
         <v>-0.39902417875182328</v>
       </c>
     </row>
-    <row r="32" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D32" s="1">
         <v>1</v>
       </c>
@@ -4388,7 +4380,7 @@
         <v>-0.34104630662549001</v>
       </c>
     </row>
-    <row r="33" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D33" s="1">
         <v>1.1000000000000001</v>
       </c>
@@ -4405,7 +4397,7 @@
         <v>-0.27624750836664685</v>
       </c>
     </row>
-    <row r="34" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D34" s="1">
         <v>1.2</v>
       </c>
@@ -4422,7 +4414,7 @@
         <v>-0.21826963624031365</v>
       </c>
     </row>
-    <row r="35" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D35" s="1">
         <v>1.3</v>
       </c>
@@ -4439,7 +4431,7 @@
         <v>-0.16711269024649009</v>
       </c>
     </row>
-    <row r="36" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D36" s="1">
         <v>1.4</v>
       </c>
@@ -4456,7 +4448,7 @@
         <v>-0.12277667038517644</v>
       </c>
     </row>
-    <row r="37" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D37" s="1">
         <v>1.5</v>
       </c>
@@ -4473,7 +4465,7 @@
         <v>-8.5261576656372504E-2</v>
       </c>
     </row>
-    <row r="38" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D38" s="1">
         <v>1.6</v>
       </c>
@@ -4490,7 +4482,7 @@
         <v>-5.4567409060078377E-2</v>
       </c>
     </row>
-    <row r="39" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D39" s="1">
         <v>1.7</v>
       </c>
@@ -4507,7 +4499,7 @@
         <v>-3.0694167596294109E-2</v>
       </c>
     </row>
-    <row r="40" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D40" s="1">
         <v>1.8</v>
       </c>
@@ -4524,7 +4516,7 @@
         <v>-1.3641852265019594E-2</v>
       </c>
     </row>
-    <row r="41" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D41" s="1">
         <v>1.9</v>
       </c>
@@ -4541,7 +4533,7 @@
         <v>-3.4104630662549059E-3</v>
       </c>
     </row>
-    <row r="42" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D42" s="1">
         <v>2</v>
       </c>
@@ -4572,14 +4564,14 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>100</v>
       </c>
@@ -4597,7 +4589,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>-40</v>
       </c>
@@ -4615,7 +4607,7 @@
         <v>-36400</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -4633,7 +4625,7 @@
         <v>-3456000</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -4642,7 +4634,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>B10</f>
         <v>40</v>
@@ -4654,7 +4646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0</v>
       </c>
@@ -4666,7 +4658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0</v>
       </c>
@@ -4678,12 +4670,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" ref="A16:C18" si="0">A6-A11</f>
         <v>60</v>
@@ -4704,7 +4696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>-40</v>
@@ -4733,7 +4725,7 @@
         <v>41200</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4765,17 +4757,17 @@
   <dimension ref="A1:T204"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="12" width="9.6328125" customWidth="1"/>
-    <col min="13" max="13" width="5.08984375" customWidth="1"/>
-    <col min="14" max="16" width="9.6328125" customWidth="1"/>
+    <col min="10" max="12" width="9.5703125" customWidth="1"/>
+    <col min="13" max="13" width="5.140625" customWidth="1"/>
+    <col min="14" max="16" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>42</v>
       </c>
@@ -4814,7 +4806,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E2" s="5">
         <v>3</v>
       </c>
@@ -4849,7 +4841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E3" s="5">
         <v>2</v>
       </c>
@@ -4881,7 +4873,7 @@
         <v>0.1368577101552777</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E4" s="5">
         <v>1</v>
       </c>
@@ -4913,7 +4905,7 @@
         <v>0.2737154203105554</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="S5">
         <f t="shared" si="1"/>
         <v>-29.167603807643381</v>
@@ -4923,7 +4915,7 @@
         <v>0.41057313046583355</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E6" t="s">
         <v>44</v>
       </c>
@@ -4951,7 +4943,7 @@
         <v>0.54743084062111125</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E7">
         <f>E2+G2*$H$2</f>
         <v>3.0001000000000002</v>
@@ -4970,11 +4962,11 @@
       </c>
       <c r="J7" s="23">
         <f>E17</f>
-        <v>10.722534602547793</v>
+        <v>11</v>
       </c>
       <c r="K7" s="24">
         <f>F17</f>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="L7" s="25">
         <f>G17</f>
@@ -5001,7 +4993,7 @@
         <v>0.68428855077638939</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E8">
         <f>E3+G3*$H$2</f>
         <v>2.0002</v>
@@ -5020,11 +5012,11 @@
       </c>
       <c r="J8" s="26">
         <f>K7</f>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="K8" s="27">
         <f>F18</f>
-        <v>10.722534602547791</v>
+        <v>8</v>
       </c>
       <c r="L8" s="28">
         <f>G18</f>
@@ -5051,7 +5043,7 @@
         <v>0.82114626093166709</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E9">
         <f>E4+G4*$H$2</f>
         <v>0.99985000000000002</v>
@@ -5078,7 +5070,7 @@
       </c>
       <c r="L9" s="31">
         <f>G19</f>
-        <v>10.722534602547791</v>
+        <v>10</v>
       </c>
       <c r="N9">
         <f t="shared" si="3"/>
@@ -5101,7 +5093,7 @@
         <v>0.95800397108694479</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="S10">
         <f t="shared" si="1"/>
         <v>-24.167603807643381</v>
@@ -5111,7 +5103,7 @@
         <v>1.0948616812422225</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
         <v>36</v>
       </c>
@@ -5120,7 +5112,7 @@
       </c>
       <c r="K11">
         <f>(J7+K8+L9)/3</f>
-        <v>10.722534602547791</v>
+        <v>9.6666666666666661</v>
       </c>
       <c r="N11" t="s">
         <v>34</v>
@@ -5138,7 +5130,7 @@
         <v>1.2317193913975002</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E12">
         <f>G7/H7</f>
         <v>3.3332222259327936E-3</v>
@@ -5156,7 +5148,7 @@
       </c>
       <c r="O12">
         <f>SUMPRODUCT(J14:L16,N7:P9)</f>
-        <v>0</v>
+        <v>-4.0553342981633628E-2</v>
       </c>
       <c r="S12">
         <f t="shared" si="1"/>
@@ -5167,7 +5159,7 @@
         <v>1.3685771015527779</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E13">
         <f>G8/H7</f>
         <v>6.6664444518507848E-3</v>
@@ -5186,9 +5178,9 @@
       <c r="N13" t="s">
         <v>28</v>
       </c>
-      <c r="O13" s="10" t="e">
+      <c r="O13" s="10">
         <f>(3*N1*O11+(N3/K19)*O12)/N3</f>
-        <v>#DIV/0!</v>
+        <v>-1.6114264794640717E-2</v>
       </c>
       <c r="S13">
         <f t="shared" si="1"/>
@@ -5199,7 +5191,7 @@
         <v>1.505434811708056</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E14">
         <f>G9/H7</f>
         <v>-4.9998333388880881E-3</v>
@@ -5214,11 +5206,11 @@
       </c>
       <c r="J14">
         <f>J7-K11</f>
-        <v>0</v>
+        <v>1.3333333333333339</v>
       </c>
       <c r="K14">
         <f>K7</f>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="L14">
         <f>L7</f>
@@ -5233,14 +5225,14 @@
         <v>1.6422925218633337</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="J15">
         <f>J8</f>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="K15">
         <f>K8-K11</f>
-        <v>0</v>
+        <v>-1.6666666666666661</v>
       </c>
       <c r="L15">
         <f>L8</f>
@@ -5249,9 +5241,9 @@
       <c r="N15" t="s">
         <v>41</v>
       </c>
-      <c r="O15" s="9" t="e">
+      <c r="O15" s="9">
         <f>$O$13*$N$3/$K$19</f>
-        <v>#DIV/0!</v>
+        <v>-4802.369654433538</v>
       </c>
       <c r="S15">
         <f t="shared" si="1"/>
@@ -5262,7 +5254,7 @@
         <v>1.7791502320186114</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E16" t="s">
         <v>6</v>
       </c>
@@ -5276,15 +5268,15 @@
       </c>
       <c r="L16">
         <f>L9-K11</f>
-        <v>0</v>
-      </c>
-      <c r="N16" s="13" t="e">
+        <v>0.33333333333333393</v>
+      </c>
+      <c r="N16" s="13">
         <f>$O$13*$N$3/$K$19/J14</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O16" s="13" t="e">
+        <v>-3601.7772408251517</v>
+      </c>
+      <c r="O16" s="13">
         <f>$O$13*$N$3/$K$19/K14</f>
-        <v>#DIV/0!</v>
+        <v>2401.184827216769</v>
       </c>
       <c r="P16" s="13" t="e">
         <f>$O$13*$N$3/$K$19/L14</f>
@@ -5299,23 +5291,23 @@
         <v>1.9160079421738891</v>
       </c>
     </row>
-    <row r="17" spans="5:20" x14ac:dyDescent="0.35">
+    <row r="17" spans="5:20" x14ac:dyDescent="0.25">
       <c r="E17" s="17">
-        <v>10.722534602547793</v>
+        <v>11</v>
       </c>
       <c r="F17" s="18">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="G17" s="19">
         <v>0</v>
       </c>
-      <c r="N17" s="9" t="e">
+      <c r="N17" s="9">
         <f>O16</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O17" s="13" t="e">
+        <v>2401.184827216769</v>
+      </c>
+      <c r="O17" s="13">
         <f>$O$13*$N$3/$K$19/K15</f>
-        <v>#DIV/0!</v>
+        <v>2881.4217926601236</v>
       </c>
       <c r="P17" s="13" t="e">
         <f>$O$13*$N$3/$K$19/L15</f>
@@ -5330,12 +5322,12 @@
         <v>2.0528656523291668</v>
       </c>
     </row>
-    <row r="18" spans="5:20" x14ac:dyDescent="0.35">
+    <row r="18" spans="5:20" x14ac:dyDescent="0.25">
       <c r="E18" s="14">
         <v>0</v>
       </c>
       <c r="F18" s="20">
-        <v>10.722534602547791</v>
+        <v>8</v>
       </c>
       <c r="G18" s="21">
         <v>0</v>
@@ -5345,7 +5337,7 @@
       </c>
       <c r="K18">
         <f>-(J7+K8+L9)</f>
-        <v>-32.167603807643374</v>
+        <v>-29</v>
       </c>
       <c r="N18" s="9" t="e">
         <f>P16</f>
@@ -5355,9 +5347,9 @@
         <f>P17</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="P18" s="13" t="e">
+      <c r="P18" s="13">
         <f>$O$13*$N$3/$K$19/L16</f>
-        <v>#DIV/0!</v>
+        <v>-14407.108963300589</v>
       </c>
       <c r="S18">
         <f t="shared" si="1"/>
@@ -5368,7 +5360,7 @@
         <v>2.189723362484445</v>
       </c>
     </row>
-    <row r="19" spans="5:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="5:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E19" s="15">
         <v>0</v>
       </c>
@@ -5376,14 +5368,14 @@
         <v>0</v>
       </c>
       <c r="G19" s="22">
-        <v>10.722534602547791</v>
+        <v>10</v>
       </c>
       <c r="J19" t="s">
         <v>19</v>
       </c>
       <c r="K19" s="3">
         <f>SQRT(0.5*SUMPRODUCT(J14:L16,J14:L16))</f>
-        <v>0</v>
+        <v>2.5166114784235831</v>
       </c>
       <c r="N19" s="10"/>
       <c r="O19" s="10"/>
@@ -5397,7 +5389,7 @@
         <v>2.3265810726397227</v>
       </c>
     </row>
-    <row r="20" spans="5:20" x14ac:dyDescent="0.35">
+    <row r="20" spans="5:20" x14ac:dyDescent="0.25">
       <c r="S20">
         <f t="shared" si="1"/>
         <v>-14.167603807643381</v>
@@ -5407,13 +5399,13 @@
         <v>2.4634387827950004</v>
       </c>
     </row>
-    <row r="21" spans="5:20" x14ac:dyDescent="0.35">
+    <row r="21" spans="5:20" x14ac:dyDescent="0.25">
       <c r="J21" s="11" t="s">
         <v>20</v>
       </c>
       <c r="K21" s="12">
         <f>K19-$N$1*K18-$N$2</f>
-        <v>0</v>
+        <v>2.0831004746303705</v>
       </c>
       <c r="S21">
         <f t="shared" si="1"/>
@@ -5424,7 +5416,7 @@
         <v>2.6002964929502781</v>
       </c>
     </row>
-    <row r="22" spans="5:20" x14ac:dyDescent="0.35">
+    <row r="22" spans="5:20" x14ac:dyDescent="0.25">
       <c r="S22">
         <f t="shared" si="1"/>
         <v>-12.167603807643381</v>
@@ -5434,7 +5426,7 @@
         <v>2.7371542031055558</v>
       </c>
     </row>
-    <row r="23" spans="5:20" x14ac:dyDescent="0.35">
+    <row r="23" spans="5:20" x14ac:dyDescent="0.25">
       <c r="J23" t="s">
         <v>23</v>
       </c>
@@ -5447,7 +5439,7 @@
       </c>
       <c r="O23" s="6">
         <f>IF(K18*$N$1+$N$2&lt;$K$19,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S23">
         <f t="shared" si="1"/>
@@ -5458,13 +5450,13 @@
         <v>2.8740119132608335</v>
       </c>
     </row>
-    <row r="24" spans="5:20" x14ac:dyDescent="0.35">
+    <row r="24" spans="5:20" x14ac:dyDescent="0.25">
       <c r="N24" t="s">
         <v>27</v>
       </c>
-      <c r="O24" s="4" t="e">
+      <c r="O24" s="4">
         <f>(K18*N1+N2)/K19</f>
-        <v>#DIV/0!</v>
+        <v>0.17225980550035713</v>
       </c>
       <c r="S24">
         <f t="shared" si="1"/>
@@ -5475,7 +5467,7 @@
         <v>3.0108696234161112</v>
       </c>
     </row>
-    <row r="25" spans="5:20" x14ac:dyDescent="0.35">
+    <row r="25" spans="5:20" x14ac:dyDescent="0.25">
       <c r="J25" t="s">
         <v>25</v>
       </c>
@@ -5491,30 +5483,30 @@
         <v>3.1477273335713893</v>
       </c>
     </row>
-    <row r="26" spans="5:20" x14ac:dyDescent="0.35">
+    <row r="26" spans="5:20" x14ac:dyDescent="0.25">
       <c r="J26" s="32">
         <f>J7-(-$K$18-$N$2/$N$1)/3</f>
-        <v>10.722534602547794</v>
+        <v>12.055867935881126</v>
       </c>
       <c r="K26" s="32">
         <f t="shared" ref="K26:L26" si="4">K7</f>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="L26" s="32">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="N26" s="32" t="e">
+      <c r="N26" s="32">
         <f>$O$24*J14-$K$18/3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O26" s="32" t="e">
+        <v>9.8963464073338088</v>
+      </c>
+      <c r="O26" s="32">
         <f>$O$24*K7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P26" s="32" t="e">
+        <v>-0.34451961100071427</v>
+      </c>
+      <c r="P26" s="32">
         <f>$O$24*L7</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="S26">
         <f t="shared" si="1"/>
@@ -5525,30 +5517,30 @@
         <v>3.284585043726667</v>
       </c>
     </row>
-    <row r="27" spans="5:20" x14ac:dyDescent="0.35">
+    <row r="27" spans="5:20" x14ac:dyDescent="0.25">
       <c r="J27" s="10">
         <f>K26</f>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="K27" s="32">
         <f>K8-(-$K$18-$N$2/$N$1)/3</f>
-        <v>10.722534602547793</v>
+        <v>9.0558679358811265</v>
       </c>
       <c r="L27" s="32">
         <f t="shared" ref="L27" si="5">L8</f>
         <v>0</v>
       </c>
-      <c r="N27" s="10" t="e">
+      <c r="N27" s="10">
         <f>O26</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O27" s="32" t="e">
+        <v>-0.34451961100071427</v>
+      </c>
+      <c r="O27" s="32">
         <f>$O$24*K15-$K$18/3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P27" s="32" t="e">
+        <v>9.3795669908327373</v>
+      </c>
+      <c r="P27" s="32">
         <f>$O$24*L8</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="S27">
         <f t="shared" si="1"/>
@@ -5559,7 +5551,7 @@
         <v>3.4214427538819447</v>
       </c>
     </row>
-    <row r="28" spans="5:20" x14ac:dyDescent="0.35">
+    <row r="28" spans="5:20" x14ac:dyDescent="0.25">
       <c r="J28" s="10">
         <f>L26</f>
         <v>0</v>
@@ -5570,19 +5562,19 @@
       </c>
       <c r="L28" s="32">
         <f>L9-(-$K$18-$N$2/$N$1)/3</f>
-        <v>10.722534602547793</v>
-      </c>
-      <c r="N28" s="10" t="e">
+        <v>11.055867935881126</v>
+      </c>
+      <c r="N28" s="10">
         <f>P26</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O28" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="O28" s="10">
         <f>P27</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P28" s="32" t="e">
+        <v>0</v>
+      </c>
+      <c r="P28" s="32">
         <f>$O$24*L16-$K$18/3</f>
-        <v>#DIV/0!</v>
+        <v>9.7240866018334522</v>
       </c>
       <c r="S28">
         <f t="shared" si="1"/>
@@ -5593,7 +5585,7 @@
         <v>3.5583004640372229</v>
       </c>
     </row>
-    <row r="29" spans="5:20" x14ac:dyDescent="0.35">
+    <row r="29" spans="5:20" x14ac:dyDescent="0.25">
       <c r="S29">
         <f t="shared" si="1"/>
         <v>-5.1676038076433812</v>
@@ -5603,20 +5595,20 @@
         <v>3.6951581741925006</v>
       </c>
     </row>
-    <row r="30" spans="5:20" x14ac:dyDescent="0.35">
+    <row r="30" spans="5:20" x14ac:dyDescent="0.25">
       <c r="J30" t="s">
         <v>10</v>
       </c>
       <c r="K30">
         <f>(J26+K27+L28)/3</f>
-        <v>10.722534602547791</v>
+        <v>10.722534602547794</v>
       </c>
       <c r="N30" t="s">
         <v>10</v>
       </c>
-      <c r="O30" t="e">
+      <c r="O30">
         <f>(N26+O27+P28)/3</f>
-        <v>#DIV/0!</v>
+        <v>9.6666666666666661</v>
       </c>
       <c r="S30">
         <f t="shared" si="1"/>
@@ -5627,7 +5619,7 @@
         <v>3.8320158843477783</v>
       </c>
     </row>
-    <row r="31" spans="5:20" x14ac:dyDescent="0.35">
+    <row r="31" spans="5:20" x14ac:dyDescent="0.25">
       <c r="S31">
         <f t="shared" si="1"/>
         <v>-3.1676038076433812</v>
@@ -5637,7 +5629,7 @@
         <v>3.968873594503056</v>
       </c>
     </row>
-    <row r="32" spans="5:20" x14ac:dyDescent="0.35">
+    <row r="32" spans="5:20" x14ac:dyDescent="0.25">
       <c r="J32" t="s">
         <v>17</v>
       </c>
@@ -5653,30 +5645,30 @@
         <v>4.1057313046583337</v>
       </c>
     </row>
-    <row r="33" spans="10:20" x14ac:dyDescent="0.35">
+    <row r="33" spans="10:20" x14ac:dyDescent="0.25">
       <c r="J33">
         <f>J26-K30</f>
-        <v>0</v>
+        <v>1.3333333333333321</v>
       </c>
       <c r="K33">
         <f>K26</f>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="L33">
         <f>L26</f>
         <v>0</v>
       </c>
-      <c r="N33" t="e">
+      <c r="N33">
         <f>N26-O30</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O33" t="e">
+        <v>0.2296797406671427</v>
+      </c>
+      <c r="O33">
         <f>O26</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P33" t="e">
+        <v>-0.34451961100071427</v>
+      </c>
+      <c r="P33">
         <f>P26</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="S33">
         <f t="shared" si="1"/>
@@ -5687,30 +5679,30 @@
         <v>4.2425890148136114</v>
       </c>
     </row>
-    <row r="34" spans="10:20" x14ac:dyDescent="0.35">
+    <row r="34" spans="10:20" x14ac:dyDescent="0.25">
       <c r="J34">
         <f>J27</f>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="K34">
         <f>K27-K30</f>
-        <v>0</v>
+        <v>-1.6666666666666679</v>
       </c>
       <c r="L34">
         <f>L27</f>
         <v>0</v>
       </c>
-      <c r="N34" t="e">
+      <c r="N34">
         <f>N27</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O34" t="e">
+        <v>-0.34451961100071427</v>
+      </c>
+      <c r="O34">
         <f>O27-O30</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P34" t="e">
+        <v>-0.28709967583392881</v>
+      </c>
+      <c r="P34">
         <f>P27</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="S34">
         <f t="shared" si="1"/>
@@ -5721,7 +5713,7 @@
         <v>4.3794467249688891</v>
       </c>
     </row>
-    <row r="35" spans="10:20" x14ac:dyDescent="0.35">
+    <row r="35" spans="10:20" x14ac:dyDescent="0.25">
       <c r="J35">
         <f>J28</f>
         <v>0</v>
@@ -5732,19 +5724,19 @@
       </c>
       <c r="L35">
         <f>L28-K30</f>
+        <v>0.33333333333333215</v>
+      </c>
+      <c r="N35">
+        <f>N28</f>
         <v>0</v>
       </c>
-      <c r="N35" t="e">
-        <f>N28</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O35" t="e">
+      <c r="O35">
         <f>O28</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P35" t="e">
+        <v>0</v>
+      </c>
+      <c r="P35">
         <f>P28-O30</f>
-        <v>#DIV/0!</v>
+        <v>5.7419935166786118E-2</v>
       </c>
       <c r="S35">
         <f t="shared" si="1"/>
@@ -5755,7 +5747,7 @@
         <v>4.5163044351241668</v>
       </c>
     </row>
-    <row r="36" spans="10:20" x14ac:dyDescent="0.35">
+    <row r="36" spans="10:20" x14ac:dyDescent="0.25">
       <c r="S36">
         <f t="shared" si="1"/>
         <v>1.8323961923566188</v>
@@ -5765,20 +5757,20 @@
         <v>4.6531621452794454</v>
       </c>
     </row>
-    <row r="37" spans="10:20" x14ac:dyDescent="0.35">
+    <row r="37" spans="10:20" x14ac:dyDescent="0.25">
       <c r="J37" s="2" t="s">
         <v>18</v>
       </c>
       <c r="K37">
         <f>-(J26+K27+L28)</f>
-        <v>-32.167603807643374</v>
+        <v>-32.167603807643381</v>
       </c>
       <c r="N37" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="O37" t="e">
+      <c r="O37">
         <f>-(N26+O27+P28)</f>
-        <v>#DIV/0!</v>
+        <v>-28.999999999999996</v>
       </c>
       <c r="S37">
         <f t="shared" si="1"/>
@@ -5789,20 +5781,20 @@
         <v>4.7900198554347231</v>
       </c>
     </row>
-    <row r="38" spans="10:20" x14ac:dyDescent="0.35">
+    <row r="38" spans="10:20" x14ac:dyDescent="0.25">
       <c r="J38" t="s">
         <v>19</v>
       </c>
       <c r="K38" s="3">
         <f>SQRT(0.5*SUMPRODUCT(J33:L35,J33:L35))</f>
-        <v>0</v>
+        <v>2.5166114784235836</v>
       </c>
       <c r="N38" t="s">
         <v>19</v>
       </c>
-      <c r="O38" s="3" t="e">
+      <c r="O38" s="3">
         <f>SQRT(0.5*SUMPRODUCT(N33:P35,N33:P35))</f>
-        <v>#DIV/0!</v>
+        <v>0.43351100379321272</v>
       </c>
       <c r="S38">
         <f t="shared" si="1"/>
@@ -5813,7 +5805,7 @@
         <v>4.9268775655900008</v>
       </c>
     </row>
-    <row r="39" spans="10:20" x14ac:dyDescent="0.35">
+    <row r="39" spans="10:20" x14ac:dyDescent="0.25">
       <c r="S39">
         <f t="shared" si="1"/>
         <v>4.8323961923566188</v>
@@ -5823,20 +5815,20 @@
         <v>5.0637352757452785</v>
       </c>
     </row>
-    <row r="40" spans="10:20" x14ac:dyDescent="0.35">
+    <row r="40" spans="10:20" x14ac:dyDescent="0.25">
       <c r="J40" t="s">
         <v>20</v>
       </c>
       <c r="K40" s="7">
         <f>K38-$N$1*K37-$N$2</f>
-        <v>0</v>
+        <v>2.5166114784235836</v>
       </c>
       <c r="N40" t="s">
         <v>20</v>
       </c>
-      <c r="O40" s="7" t="e">
+      <c r="O40" s="7">
         <f>O38-$N$1*O37-$N$2</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="S40">
         <f t="shared" si="1"/>
@@ -5847,7 +5839,7 @@
         <v>5.2005929859005562</v>
       </c>
     </row>
-    <row r="41" spans="10:20" x14ac:dyDescent="0.35">
+    <row r="41" spans="10:20" x14ac:dyDescent="0.25">
       <c r="S41">
         <f t="shared" si="1"/>
         <v>6.8323961923566188</v>
@@ -5857,7 +5849,7 @@
         <v>5.3374506960558339</v>
       </c>
     </row>
-    <row r="42" spans="10:20" x14ac:dyDescent="0.35">
+    <row r="42" spans="10:20" x14ac:dyDescent="0.25">
       <c r="J42" t="s">
         <v>23</v>
       </c>
@@ -5868,9 +5860,9 @@
       <c r="N42" t="s">
         <v>24</v>
       </c>
-      <c r="O42" t="e">
+      <c r="O42">
         <f>IF(O37*$N$1+$N$2&lt;$O$38,1,0)</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="S42">
         <f t="shared" si="1"/>
@@ -5881,7 +5873,7 @@
         <v>5.4743084062111116</v>
       </c>
     </row>
-    <row r="43" spans="10:20" x14ac:dyDescent="0.35">
+    <row r="43" spans="10:20" x14ac:dyDescent="0.25">
       <c r="S43">
         <f t="shared" si="1"/>
         <v>8.8323961923566188</v>
@@ -5891,7 +5883,7 @@
         <v>5.6111661163663893</v>
       </c>
     </row>
-    <row r="44" spans="10:20" x14ac:dyDescent="0.35">
+    <row r="44" spans="10:20" x14ac:dyDescent="0.25">
       <c r="S44">
         <f t="shared" si="1"/>
         <v>9.8323961923566188</v>
@@ -5901,7 +5893,7 @@
         <v>5.748023826521667</v>
       </c>
     </row>
-    <row r="45" spans="10:20" x14ac:dyDescent="0.35">
+    <row r="45" spans="10:20" x14ac:dyDescent="0.25">
       <c r="S45">
         <f t="shared" si="1"/>
         <v>10.832396192356619</v>
@@ -5911,7 +5903,7 @@
         <v>5.8848815366769447</v>
       </c>
     </row>
-    <row r="46" spans="10:20" x14ac:dyDescent="0.35">
+    <row r="46" spans="10:20" x14ac:dyDescent="0.25">
       <c r="S46">
         <f t="shared" si="1"/>
         <v>11.832396192356619</v>
@@ -5921,7 +5913,7 @@
         <v>6.0217392468322224</v>
       </c>
     </row>
-    <row r="47" spans="10:20" x14ac:dyDescent="0.35">
+    <row r="47" spans="10:20" x14ac:dyDescent="0.25">
       <c r="S47">
         <f t="shared" si="1"/>
         <v>12.832396192356619</v>
@@ -5931,7 +5923,7 @@
         <v>6.1585969569875001</v>
       </c>
     </row>
-    <row r="48" spans="10:20" x14ac:dyDescent="0.35">
+    <row r="48" spans="10:20" x14ac:dyDescent="0.25">
       <c r="S48">
         <f t="shared" si="1"/>
         <v>13.832396192356619</v>
@@ -5941,7 +5933,7 @@
         <v>6.2954546671427778</v>
       </c>
     </row>
-    <row r="49" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="49" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S49">
         <f t="shared" si="1"/>
         <v>14.832396192356619</v>
@@ -5951,7 +5943,7 @@
         <v>6.4323123772980555</v>
       </c>
     </row>
-    <row r="50" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="50" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S50">
         <f t="shared" si="1"/>
         <v>15.832396192356619</v>
@@ -5961,7 +5953,7 @@
         <v>6.5691700874533341</v>
       </c>
     </row>
-    <row r="51" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="51" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S51">
         <f t="shared" si="1"/>
         <v>16.832396192356619</v>
@@ -5971,7 +5963,7 @@
         <v>6.7060277976086118</v>
       </c>
     </row>
-    <row r="52" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="52" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S52">
         <f t="shared" si="1"/>
         <v>17.832396192356619</v>
@@ -5981,7 +5973,7 @@
         <v>6.8428855077638895</v>
       </c>
     </row>
-    <row r="53" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="53" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S53">
         <f t="shared" si="1"/>
         <v>18.832396192356619</v>
@@ -5991,7 +5983,7 @@
         <v>6.9797432179191672</v>
       </c>
     </row>
-    <row r="54" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="54" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S54">
         <f t="shared" si="1"/>
         <v>19.832396192356619</v>
@@ -6001,7 +5993,7 @@
         <v>7.1166009280744449</v>
       </c>
     </row>
-    <row r="55" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="55" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S55">
         <f t="shared" si="1"/>
         <v>20.832396192356619</v>
@@ -6011,7 +6003,7 @@
         <v>7.2534586382297235</v>
       </c>
     </row>
-    <row r="56" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="56" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S56">
         <f t="shared" si="1"/>
         <v>21.832396192356619</v>
@@ -6021,7 +6013,7 @@
         <v>7.3903163483850012</v>
       </c>
     </row>
-    <row r="57" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="57" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S57">
         <f t="shared" si="1"/>
         <v>22.832396192356619</v>
@@ -6031,7 +6023,7 @@
         <v>7.5271740585402789</v>
       </c>
     </row>
-    <row r="58" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="58" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S58">
         <f t="shared" si="1"/>
         <v>23.832396192356619</v>
@@ -6041,7 +6033,7 @@
         <v>7.6640317686955566</v>
       </c>
     </row>
-    <row r="59" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="59" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S59">
         <f t="shared" si="1"/>
         <v>24.832396192356619</v>
@@ -6051,7 +6043,7 @@
         <v>7.8008894788508343</v>
       </c>
     </row>
-    <row r="60" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="60" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S60">
         <f t="shared" si="1"/>
         <v>25.832396192356619</v>
@@ -6061,7 +6053,7 @@
         <v>7.937747189006112</v>
       </c>
     </row>
-    <row r="61" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="61" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S61">
         <f t="shared" si="1"/>
         <v>26.832396192356619</v>
@@ -6071,7 +6063,7 @@
         <v>8.0746048991613897</v>
       </c>
     </row>
-    <row r="62" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="62" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S62">
         <f t="shared" si="1"/>
         <v>27.832396192356619</v>
@@ -6081,7 +6073,7 @@
         <v>8.2114626093166674</v>
       </c>
     </row>
-    <row r="63" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="63" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S63">
         <f t="shared" si="1"/>
         <v>28.832396192356619</v>
@@ -6091,7 +6083,7 @@
         <v>8.3483203194719451</v>
       </c>
     </row>
-    <row r="64" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="64" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S64">
         <f t="shared" si="1"/>
         <v>29.832396192356619</v>
@@ -6101,7 +6093,7 @@
         <v>8.4851780296272228</v>
       </c>
     </row>
-    <row r="65" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="65" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S65">
         <f t="shared" si="1"/>
         <v>30.832396192356619</v>
@@ -6111,7 +6103,7 @@
         <v>8.6220357397825005</v>
       </c>
     </row>
-    <row r="66" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="66" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S66">
         <f t="shared" si="1"/>
         <v>31.832396192356619</v>
@@ -6121,7 +6113,7 @@
         <v>8.7588934499377782</v>
       </c>
     </row>
-    <row r="67" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="67" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S67">
         <f t="shared" si="1"/>
         <v>32.832396192356619</v>
@@ -6131,7 +6123,7 @@
         <v>8.8957511600930559</v>
       </c>
     </row>
-    <row r="68" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="68" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S68">
         <f t="shared" ref="S68:S131" si="7">S67+1</f>
         <v>33.832396192356619</v>
@@ -6141,7 +6133,7 @@
         <v>9.0326088702483336</v>
       </c>
     </row>
-    <row r="69" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="69" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S69">
         <f t="shared" si="7"/>
         <v>34.832396192356619</v>
@@ -6151,7 +6143,7 @@
         <v>9.1694665804036113</v>
       </c>
     </row>
-    <row r="70" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="70" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S70">
         <f t="shared" si="7"/>
         <v>35.832396192356619</v>
@@ -6161,7 +6153,7 @@
         <v>9.3063242905588908</v>
       </c>
     </row>
-    <row r="71" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="71" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S71">
         <f t="shared" si="7"/>
         <v>36.832396192356619</v>
@@ -6171,7 +6163,7 @@
         <v>9.4431820007141667</v>
       </c>
     </row>
-    <row r="72" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="72" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S72">
         <f t="shared" si="7"/>
         <v>37.832396192356619</v>
@@ -6181,7 +6173,7 @@
         <v>9.5800397108694462</v>
       </c>
     </row>
-    <row r="73" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="73" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S73">
         <f t="shared" si="7"/>
         <v>38.832396192356619</v>
@@ -6191,7 +6183,7 @@
         <v>9.7168974210247221</v>
       </c>
     </row>
-    <row r="74" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="74" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S74">
         <f t="shared" si="7"/>
         <v>39.832396192356619</v>
@@ -6201,7 +6193,7 @@
         <v>9.8537551311800016</v>
       </c>
     </row>
-    <row r="75" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="75" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S75">
         <f t="shared" si="7"/>
         <v>40.832396192356619</v>
@@ -6211,7 +6203,7 @@
         <v>9.9906128413352775</v>
       </c>
     </row>
-    <row r="76" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="76" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S76">
         <f t="shared" si="7"/>
         <v>41.832396192356619</v>
@@ -6221,7 +6213,7 @@
         <v>10.127470551490557</v>
       </c>
     </row>
-    <row r="77" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="77" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S77">
         <f t="shared" si="7"/>
         <v>42.832396192356619</v>
@@ -6231,7 +6223,7 @@
         <v>10.264328261645833</v>
       </c>
     </row>
-    <row r="78" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="78" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S78">
         <f t="shared" si="7"/>
         <v>43.832396192356619</v>
@@ -6241,7 +6233,7 @@
         <v>10.401185971801112</v>
       </c>
     </row>
-    <row r="79" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="79" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S79">
         <f t="shared" si="7"/>
         <v>44.832396192356619</v>
@@ -6251,7 +6243,7 @@
         <v>10.53804368195639</v>
       </c>
     </row>
-    <row r="80" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="80" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S80">
         <f t="shared" si="7"/>
         <v>45.832396192356619</v>
@@ -6261,7 +6253,7 @@
         <v>10.674901392111668</v>
       </c>
     </row>
-    <row r="81" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="81" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S81">
         <f t="shared" si="7"/>
         <v>46.832396192356619</v>
@@ -6271,7 +6263,7 @@
         <v>10.811759102266945</v>
       </c>
     </row>
-    <row r="82" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="82" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S82">
         <f t="shared" si="7"/>
         <v>47.832396192356619</v>
@@ -6281,7 +6273,7 @@
         <v>10.948616812422223</v>
       </c>
     </row>
-    <row r="83" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="83" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S83">
         <f t="shared" si="7"/>
         <v>48.832396192356619</v>
@@ -6291,7 +6283,7 @@
         <v>11.085474522577501</v>
       </c>
     </row>
-    <row r="84" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="84" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S84">
         <f t="shared" si="7"/>
         <v>49.832396192356619</v>
@@ -6301,7 +6293,7 @@
         <v>11.222332232732779</v>
       </c>
     </row>
-    <row r="85" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="85" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S85">
         <f t="shared" si="7"/>
         <v>50.832396192356619</v>
@@ -6311,7 +6303,7 @@
         <v>11.359189942888056</v>
       </c>
     </row>
-    <row r="86" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="86" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S86">
         <f t="shared" si="7"/>
         <v>51.832396192356619</v>
@@ -6321,7 +6313,7 @@
         <v>11.496047653043334</v>
       </c>
     </row>
-    <row r="87" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="87" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S87">
         <f t="shared" si="7"/>
         <v>52.832396192356619</v>
@@ -6331,7 +6323,7 @@
         <v>11.632905363198612</v>
       </c>
     </row>
-    <row r="88" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="88" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S88">
         <f t="shared" si="7"/>
         <v>53.832396192356619</v>
@@ -6341,7 +6333,7 @@
         <v>11.769763073353889</v>
       </c>
     </row>
-    <row r="89" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="89" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S89">
         <f t="shared" si="7"/>
         <v>54.832396192356619</v>
@@ -6351,7 +6343,7 @@
         <v>11.906620783509167</v>
       </c>
     </row>
-    <row r="90" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="90" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S90">
         <f t="shared" si="7"/>
         <v>55.832396192356619</v>
@@ -6361,7 +6353,7 @@
         <v>12.043478493664445</v>
       </c>
     </row>
-    <row r="91" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="91" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S91">
         <f t="shared" si="7"/>
         <v>56.832396192356619</v>
@@ -6371,7 +6363,7 @@
         <v>12.180336203819724</v>
       </c>
     </row>
-    <row r="92" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="92" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S92">
         <f t="shared" si="7"/>
         <v>57.832396192356619</v>
@@ -6381,7 +6373,7 @@
         <v>12.317193913975</v>
       </c>
     </row>
-    <row r="93" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="93" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S93">
         <f t="shared" si="7"/>
         <v>58.832396192356619</v>
@@ -6391,7 +6383,7 @@
         <v>12.45405162413028</v>
       </c>
     </row>
-    <row r="94" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="94" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S94">
         <f t="shared" si="7"/>
         <v>59.832396192356619</v>
@@ -6401,7 +6393,7 @@
         <v>12.590909334285556</v>
       </c>
     </row>
-    <row r="95" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="95" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S95">
         <f t="shared" si="7"/>
         <v>60.832396192356619</v>
@@ -6411,7 +6403,7 @@
         <v>12.727767044440835</v>
       </c>
     </row>
-    <row r="96" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="96" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S96">
         <f t="shared" si="7"/>
         <v>61.832396192356619</v>
@@ -6421,7 +6413,7 @@
         <v>12.864624754596111</v>
       </c>
     </row>
-    <row r="97" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="97" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S97">
         <f t="shared" si="7"/>
         <v>62.832396192356619</v>
@@ -6431,7 +6423,7 @@
         <v>13.00148246475139</v>
       </c>
     </row>
-    <row r="98" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="98" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S98">
         <f t="shared" si="7"/>
         <v>63.832396192356619</v>
@@ -6441,7 +6433,7 @@
         <v>13.138340174906666</v>
       </c>
     </row>
-    <row r="99" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="99" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S99">
         <f t="shared" si="7"/>
         <v>64.832396192356612</v>
@@ -6451,7 +6443,7 @@
         <v>13.275197885061946</v>
       </c>
     </row>
-    <row r="100" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="100" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S100">
         <f t="shared" si="7"/>
         <v>65.832396192356612</v>
@@ -6461,7 +6453,7 @@
         <v>13.412055595217222</v>
       </c>
     </row>
-    <row r="101" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="101" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S101">
         <f t="shared" si="7"/>
         <v>66.832396192356612</v>
@@ -6471,7 +6463,7 @@
         <v>13.548913305372501</v>
       </c>
     </row>
-    <row r="102" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="102" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S102">
         <f t="shared" si="7"/>
         <v>67.832396192356612</v>
@@ -6481,7 +6473,7 @@
         <v>13.685771015527777</v>
       </c>
     </row>
-    <row r="103" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="103" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S103">
         <f t="shared" si="7"/>
         <v>68.832396192356612</v>
@@ -6491,7 +6483,7 @@
         <v>13.822628725683057</v>
       </c>
     </row>
-    <row r="104" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="104" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S104">
         <f t="shared" si="7"/>
         <v>69.832396192356612</v>
@@ -6501,7 +6493,7 @@
         <v>13.959486435838333</v>
       </c>
     </row>
-    <row r="105" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="105" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S105">
         <f t="shared" si="7"/>
         <v>70.832396192356612</v>
@@ -6511,7 +6503,7 @@
         <v>14.096344145993612</v>
       </c>
     </row>
-    <row r="106" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="106" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S106">
         <f t="shared" si="7"/>
         <v>71.832396192356612</v>
@@ -6521,7 +6513,7 @@
         <v>14.233201856148888</v>
       </c>
     </row>
-    <row r="107" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="107" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S107">
         <f t="shared" si="7"/>
         <v>72.832396192356612</v>
@@ -6531,7 +6523,7 @@
         <v>14.370059566304167</v>
       </c>
     </row>
-    <row r="108" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="108" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S108">
         <f t="shared" si="7"/>
         <v>73.832396192356612</v>
@@ -6541,7 +6533,7 @@
         <v>14.506917276459443</v>
       </c>
     </row>
-    <row r="109" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="109" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S109">
         <f t="shared" si="7"/>
         <v>74.832396192356612</v>
@@ -6551,7 +6543,7 @@
         <v>14.643774986614723</v>
       </c>
     </row>
-    <row r="110" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="110" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S110">
         <f t="shared" si="7"/>
         <v>75.832396192356612</v>
@@ -6561,7 +6553,7 @@
         <v>14.780632696769999</v>
       </c>
     </row>
-    <row r="111" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="111" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S111">
         <f t="shared" si="7"/>
         <v>76.832396192356612</v>
@@ -6571,7 +6563,7 @@
         <v>14.917490406925278</v>
       </c>
     </row>
-    <row r="112" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="112" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S112">
         <f t="shared" si="7"/>
         <v>77.832396192356612</v>
@@ -6581,7 +6573,7 @@
         <v>15.054348117080554</v>
       </c>
     </row>
-    <row r="113" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="113" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S113">
         <f t="shared" si="7"/>
         <v>78.832396192356612</v>
@@ -6591,7 +6583,7 @@
         <v>15.191205827235834</v>
       </c>
     </row>
-    <row r="114" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="114" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S114">
         <f t="shared" si="7"/>
         <v>79.832396192356612</v>
@@ -6601,7 +6593,7 @@
         <v>15.32806353739111</v>
       </c>
     </row>
-    <row r="115" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="115" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S115">
         <f t="shared" si="7"/>
         <v>80.832396192356612</v>
@@ -6611,7 +6603,7 @@
         <v>15.464921247546389</v>
       </c>
     </row>
-    <row r="116" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="116" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S116">
         <f t="shared" si="7"/>
         <v>81.832396192356612</v>
@@ -6621,7 +6613,7 @@
         <v>15.601778957701665</v>
       </c>
     </row>
-    <row r="117" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="117" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S117">
         <f t="shared" si="7"/>
         <v>82.832396192356612</v>
@@ -6631,7 +6623,7 @@
         <v>15.738636667856944</v>
       </c>
     </row>
-    <row r="118" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="118" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S118">
         <f t="shared" si="7"/>
         <v>83.832396192356612</v>
@@ -6641,7 +6633,7 @@
         <v>15.875494378012224</v>
       </c>
     </row>
-    <row r="119" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="119" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S119">
         <f t="shared" si="7"/>
         <v>84.832396192356612</v>
@@ -6651,7 +6643,7 @@
         <v>16.0123520881675</v>
       </c>
     </row>
-    <row r="120" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="120" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S120">
         <f t="shared" si="7"/>
         <v>85.832396192356612</v>
@@ -6661,7 +6653,7 @@
         <v>16.149209798322779</v>
       </c>
     </row>
-    <row r="121" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="121" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S121">
         <f t="shared" si="7"/>
         <v>86.832396192356612</v>
@@ -6671,7 +6663,7 @@
         <v>16.286067508478055</v>
       </c>
     </row>
-    <row r="122" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="122" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S122">
         <f t="shared" si="7"/>
         <v>87.832396192356612</v>
@@ -6681,7 +6673,7 @@
         <v>16.422925218633335</v>
       </c>
     </row>
-    <row r="123" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="123" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S123">
         <f t="shared" si="7"/>
         <v>88.832396192356612</v>
@@ -6691,7 +6683,7 @@
         <v>16.559782928788611</v>
       </c>
     </row>
-    <row r="124" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="124" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S124">
         <f t="shared" si="7"/>
         <v>89.832396192356612</v>
@@ -6701,7 +6693,7 @@
         <v>16.69664063894389</v>
       </c>
     </row>
-    <row r="125" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="125" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S125">
         <f t="shared" si="7"/>
         <v>90.832396192356612</v>
@@ -6711,7 +6703,7 @@
         <v>16.833498349099166</v>
       </c>
     </row>
-    <row r="126" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="126" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S126">
         <f t="shared" si="7"/>
         <v>91.832396192356612</v>
@@ -6721,7 +6713,7 @@
         <v>16.970356059254446</v>
       </c>
     </row>
-    <row r="127" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="127" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S127">
         <f t="shared" si="7"/>
         <v>92.832396192356612</v>
@@ -6731,7 +6723,7 @@
         <v>17.107213769409721</v>
       </c>
     </row>
-    <row r="128" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="128" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S128">
         <f t="shared" si="7"/>
         <v>93.832396192356612</v>
@@ -6741,7 +6733,7 @@
         <v>17.244071479565001</v>
       </c>
     </row>
-    <row r="129" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="129" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S129">
         <f t="shared" si="7"/>
         <v>94.832396192356612</v>
@@ -6751,7 +6743,7 @@
         <v>17.380929189720277</v>
       </c>
     </row>
-    <row r="130" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="130" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S130">
         <f t="shared" si="7"/>
         <v>95.832396192356612</v>
@@ -6761,7 +6753,7 @@
         <v>17.517786899875556</v>
       </c>
     </row>
-    <row r="131" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="131" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S131">
         <f t="shared" si="7"/>
         <v>96.832396192356612</v>
@@ -6771,7 +6763,7 @@
         <v>17.654644610030832</v>
       </c>
     </row>
-    <row r="132" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="132" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S132">
         <f t="shared" ref="S132:S134" si="9">S131+1</f>
         <v>97.832396192356612</v>
@@ -6781,7 +6773,7 @@
         <v>17.791502320186112</v>
       </c>
     </row>
-    <row r="133" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="133" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S133">
         <f t="shared" si="9"/>
         <v>98.832396192356612</v>
@@ -6791,7 +6783,7 @@
         <v>17.928360030341388</v>
       </c>
     </row>
-    <row r="134" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="134" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S134">
         <f t="shared" si="9"/>
         <v>99.832396192356612</v>
@@ -6801,214 +6793,214 @@
         <v>18.065217740496667</v>
       </c>
     </row>
-    <row r="135" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="135" spans="19:20" x14ac:dyDescent="0.25">
       <c r="T135" s="4"/>
     </row>
-    <row r="136" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="136" spans="19:20" x14ac:dyDescent="0.25">
       <c r="T136" s="4"/>
     </row>
-    <row r="137" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="137" spans="19:20" x14ac:dyDescent="0.25">
       <c r="T137" s="4"/>
     </row>
-    <row r="138" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="138" spans="19:20" x14ac:dyDescent="0.25">
       <c r="T138" s="4"/>
     </row>
-    <row r="139" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="139" spans="19:20" x14ac:dyDescent="0.25">
       <c r="T139" s="4"/>
     </row>
-    <row r="140" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="140" spans="19:20" x14ac:dyDescent="0.25">
       <c r="T140" s="4"/>
     </row>
-    <row r="141" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="141" spans="19:20" x14ac:dyDescent="0.25">
       <c r="T141" s="4"/>
     </row>
-    <row r="142" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="142" spans="19:20" x14ac:dyDescent="0.25">
       <c r="T142" s="4"/>
     </row>
-    <row r="143" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="143" spans="19:20" x14ac:dyDescent="0.25">
       <c r="T143" s="4"/>
     </row>
-    <row r="144" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="144" spans="19:20" x14ac:dyDescent="0.25">
       <c r="T144" s="4"/>
     </row>
-    <row r="145" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="145" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T145" s="4"/>
     </row>
-    <row r="146" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="146" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T146" s="4"/>
     </row>
-    <row r="147" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="147" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T147" s="4"/>
     </row>
-    <row r="148" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="148" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T148" s="4"/>
     </row>
-    <row r="149" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="149" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T149" s="4"/>
     </row>
-    <row r="150" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="150" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T150" s="4"/>
     </row>
-    <row r="151" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="151" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T151" s="4"/>
     </row>
-    <row r="152" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="152" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T152" s="4"/>
     </row>
-    <row r="153" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="153" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T153" s="4"/>
     </row>
-    <row r="154" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="154" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T154" s="4"/>
     </row>
-    <row r="155" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="155" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T155" s="4"/>
     </row>
-    <row r="156" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="156" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T156" s="4"/>
     </row>
-    <row r="157" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="157" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T157" s="4"/>
     </row>
-    <row r="158" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="158" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T158" s="4"/>
     </row>
-    <row r="159" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="159" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T159" s="4"/>
     </row>
-    <row r="160" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="160" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T160" s="4"/>
     </row>
-    <row r="161" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="161" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T161" s="4"/>
     </row>
-    <row r="162" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="162" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T162" s="4"/>
     </row>
-    <row r="163" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="163" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T163" s="4"/>
     </row>
-    <row r="164" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="164" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T164" s="4"/>
     </row>
-    <row r="165" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="165" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T165" s="4"/>
     </row>
-    <row r="166" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="166" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T166" s="4"/>
     </row>
-    <row r="167" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="167" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T167" s="4"/>
     </row>
-    <row r="168" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="168" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T168" s="4"/>
     </row>
-    <row r="169" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="169" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T169" s="4"/>
     </row>
-    <row r="170" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="170" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T170" s="4"/>
     </row>
-    <row r="171" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="171" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T171" s="4"/>
     </row>
-    <row r="172" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="172" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T172" s="4"/>
     </row>
-    <row r="173" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="173" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T173" s="4"/>
     </row>
-    <row r="174" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="174" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T174" s="4"/>
     </row>
-    <row r="175" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="175" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T175" s="4"/>
     </row>
-    <row r="176" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="176" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T176" s="4"/>
     </row>
-    <row r="177" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="177" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T177" s="4"/>
     </row>
-    <row r="178" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="178" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T178" s="4"/>
     </row>
-    <row r="179" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="179" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T179" s="4"/>
     </row>
-    <row r="180" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="180" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T180" s="4"/>
     </row>
-    <row r="181" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="181" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T181" s="4"/>
     </row>
-    <row r="182" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="182" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T182" s="4"/>
     </row>
-    <row r="183" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="183" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T183" s="4"/>
     </row>
-    <row r="184" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="184" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T184" s="4"/>
     </row>
-    <row r="185" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="185" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T185" s="4"/>
     </row>
-    <row r="186" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="186" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T186" s="4"/>
     </row>
-    <row r="187" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="187" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T187" s="4"/>
     </row>
-    <row r="188" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="188" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T188" s="4"/>
     </row>
-    <row r="189" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="189" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T189" s="4"/>
     </row>
-    <row r="190" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="190" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T190" s="4"/>
     </row>
-    <row r="191" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="191" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T191" s="4"/>
     </row>
-    <row r="192" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="192" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T192" s="4"/>
     </row>
-    <row r="193" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="193" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T193" s="4"/>
     </row>
-    <row r="194" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="194" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T194" s="4"/>
     </row>
-    <row r="195" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="195" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T195" s="4"/>
     </row>
-    <row r="196" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="196" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T196" s="4"/>
     </row>
-    <row r="197" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="197" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T197" s="4"/>
     </row>
-    <row r="198" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="198" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T198" s="4"/>
     </row>
-    <row r="199" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="199" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T199" s="4"/>
     </row>
-    <row r="200" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="200" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T200" s="4"/>
     </row>
-    <row r="201" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="201" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T201" s="4"/>
     </row>
-    <row r="202" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="202" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T202" s="4"/>
     </row>
-    <row r="203" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="203" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T203" s="4"/>
     </row>
-    <row r="204" spans="20:20" x14ac:dyDescent="0.35">
+    <row r="204" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T204" s="4"/>
     </row>
   </sheetData>
@@ -7024,7 +7016,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
common update 01 28.04.2022
</commit_message>
<xml_diff>
--- a/data/draft.xlsx
+++ b/data/draft.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Benutzer\Lei\Documents\Git\tiSPHi\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C9F758B-0D11-45B7-87AF-2FC3A83B58EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE81B531-AE33-418A-96DE-BE439BE15300}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="25815" windowHeight="15615" activeTab="2" xr2:uid="{F96AF2A0-9E31-4557-A308-4BAF8AA6954F}"/>
   </bookViews>
@@ -1950,7 +1950,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>-32.167603807643381</c:v>
+                  <c:v>-15.299199999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1962,7 +1962,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2.3084714018876937</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4757,7 +4757,7 @@
   <dimension ref="A1:T204"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+      <selection activeCell="AB4" sqref="AB4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4966,11 +4966,11 @@
       </c>
       <c r="J7" s="23">
         <f>E17</f>
-        <v>10.722534602547794</v>
+        <v>6.2991999999999999</v>
       </c>
       <c r="K7" s="24">
         <f>F17</f>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="L7" s="25">
         <f>G17</f>
@@ -5016,11 +5016,11 @@
       </c>
       <c r="J8" s="26">
         <f>K7</f>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="K8" s="27">
         <f>F18</f>
-        <v>10.722534602547794</v>
+        <v>4</v>
       </c>
       <c r="L8" s="28">
         <f>G18</f>
@@ -5074,7 +5074,7 @@
       </c>
       <c r="L9" s="31">
         <f>G19</f>
-        <v>10.722534602547794</v>
+        <v>5</v>
       </c>
       <c r="N9">
         <f>P7</f>
@@ -5116,7 +5116,7 @@
       </c>
       <c r="K11">
         <f>(J7+K8+L9)/3</f>
-        <v>10.722534602547794</v>
+        <v>5.099733333333333</v>
       </c>
       <c r="N11" t="s">
         <v>34</v>
@@ -5152,7 +5152,7 @@
       </c>
       <c r="O12">
         <f>SUMPRODUCT(J14:L16,N7:P9)</f>
-        <v>0</v>
+        <v>-2.8833809327410222E-2</v>
       </c>
       <c r="S12">
         <f t="shared" si="1"/>
@@ -5182,9 +5182,9 @@
       <c r="N13" t="s">
         <v>28</v>
       </c>
-      <c r="O13" s="10" t="e">
+      <c r="O13" s="10">
         <f>(3*N1*O11+(N3/K19)*O12)/N3</f>
-        <v>#DIV/0!</v>
+        <v>-1.2490434149333368E-2</v>
       </c>
       <c r="S13">
         <f t="shared" si="1"/>
@@ -5210,11 +5210,11 @@
       </c>
       <c r="J14">
         <f>J7-K11</f>
-        <v>0</v>
+        <v>1.1994666666666669</v>
       </c>
       <c r="K14">
         <f>K7</f>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="L14">
         <f>L7</f>
@@ -5232,11 +5232,11 @@
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="J15">
         <f>J8</f>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="K15">
         <f>K8-K11</f>
-        <v>0</v>
+        <v>-1.099733333333333</v>
       </c>
       <c r="L15">
         <f>L8</f>
@@ -5245,9 +5245,9 @@
       <c r="N15" t="s">
         <v>41</v>
       </c>
-      <c r="O15" s="9" t="e">
+      <c r="O15" s="9">
         <f>$O$13*$N$3/$K$19</f>
-        <v>#DIV/0!</v>
+        <v>-4058.0210802437168</v>
       </c>
       <c r="S15">
         <f t="shared" si="1"/>
@@ -5272,15 +5272,15 @@
       </c>
       <c r="L16">
         <f>L9-K11</f>
-        <v>0</v>
-      </c>
-      <c r="N16" s="13" t="e">
+        <v>-9.9733333333333007E-2</v>
+      </c>
+      <c r="N16" s="13">
         <f>$O$15/J14</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O16" s="13" t="e">
+        <v>-3383.187872590915</v>
+      </c>
+      <c r="O16" s="13">
         <f t="shared" ref="O16:P16" si="3">$O$15/K14</f>
-        <v>#DIV/0!</v>
+        <v>2029.0105401218584</v>
       </c>
       <c r="P16" s="13" t="e">
         <f t="shared" si="3"/>
@@ -5306,21 +5306,21 @@
         <v>0</v>
       </c>
       <c r="E17" s="17">
-        <v>10.722534602547794</v>
+        <v>6.2991999999999999</v>
       </c>
       <c r="F17" s="18">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="G17" s="19">
         <v>0</v>
       </c>
-      <c r="N17" s="9" t="e">
+      <c r="N17" s="9">
         <f>O16</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O17" s="13" t="e">
+        <v>2029.0105401218584</v>
+      </c>
+      <c r="O17" s="13">
         <f t="shared" ref="O17" si="4">$O$15/K15</f>
-        <v>#DIV/0!</v>
+        <v>3690.0046195232644</v>
       </c>
       <c r="P17" s="13" t="e">
         <f t="shared" ref="P17:P18" si="5">$O$15/L15</f>
@@ -5349,7 +5349,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="20">
-        <v>10.722534602547794</v>
+        <v>4</v>
       </c>
       <c r="G18" s="21">
         <v>0</v>
@@ -5359,7 +5359,7 @@
       </c>
       <c r="K18">
         <f>-(J7+K8+L9)</f>
-        <v>-32.167603807643381</v>
+        <v>-15.299199999999999</v>
       </c>
       <c r="N18" s="9" t="e">
         <f>P16</f>
@@ -5369,9 +5369,9 @@
         <f>P17</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="P18" s="13" t="e">
+      <c r="P18" s="13">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>40688.71403987697</v>
       </c>
       <c r="S18">
         <f t="shared" si="1"/>
@@ -5399,14 +5399,14 @@
         <v>0</v>
       </c>
       <c r="G19" s="22">
-        <v>10.722534602547794</v>
+        <v>5</v>
       </c>
       <c r="J19" t="s">
         <v>19</v>
       </c>
       <c r="K19" s="3">
         <f>SQRT(0.5*SUMPRODUCT(J14:L16,J14:L16))</f>
-        <v>0</v>
+        <v>2.3084714018876937</v>
       </c>
       <c r="N19" s="10"/>
       <c r="O19" s="10"/>
@@ -5436,7 +5436,7 @@
       </c>
       <c r="K21" s="12">
         <f>K19-$N$1*K18-$N$2</f>
-        <v>0</v>
+        <v>-9.9717200948923335E-5</v>
       </c>
       <c r="S21">
         <f t="shared" si="1"/>
@@ -5485,9 +5485,9 @@
       <c r="N24" t="s">
         <v>27</v>
       </c>
-      <c r="O24" s="4" t="e">
+      <c r="O24" s="4">
         <f>(K18*N1+N2)/K19</f>
-        <v>#DIV/0!</v>
+        <v>1.000043196203716</v>
       </c>
       <c r="S24">
         <f t="shared" si="1"/>
@@ -5517,27 +5517,27 @@
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="J26" s="32">
         <f>J7-(-$K$18-$N$2/$N$1)/3</f>
-        <v>10.722534602547794</v>
+        <v>11.92200126921446</v>
       </c>
       <c r="K26" s="32">
         <f t="shared" ref="K26:L26" si="6">K7</f>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="L26" s="32">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="N26" s="32" t="e">
+      <c r="N26" s="32">
         <f>$O$24*J14-$K$18/3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O26" s="32" t="e">
+        <v>6.2992518124064834</v>
+      </c>
+      <c r="O26" s="32">
         <f>$O$24*K7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P26" s="32" t="e">
+        <v>-2.0000863924074319</v>
+      </c>
+      <c r="P26" s="32">
         <f>$O$24*L7</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="S26">
         <f t="shared" si="1"/>
@@ -5551,27 +5551,27 @@
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="J27" s="10">
         <f>K26</f>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="K27" s="32">
         <f>K8-(-$K$18-$N$2/$N$1)/3</f>
-        <v>10.722534602547794</v>
+        <v>9.6228012692144596</v>
       </c>
       <c r="L27" s="32">
         <f t="shared" ref="L27" si="7">L8</f>
         <v>0</v>
       </c>
-      <c r="N27" s="10" t="e">
+      <c r="N27" s="10">
         <f>O26</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O27" s="32" t="e">
+        <v>-2.0000863924074319</v>
+      </c>
+      <c r="O27" s="32">
         <f>$O$24*K15-$K$18/3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P27" s="32" t="e">
+        <v>3.9999524956949002</v>
+      </c>
+      <c r="P27" s="32">
         <f>$O$24*L8</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="S27">
         <f t="shared" si="1"/>
@@ -5593,19 +5593,19 @@
       </c>
       <c r="L28" s="32">
         <f>L9-(-$K$18-$N$2/$N$1)/3</f>
-        <v>10.722534602547794</v>
-      </c>
-      <c r="N28" s="10" t="e">
+        <v>10.62280126921446</v>
+      </c>
+      <c r="N28" s="10">
         <f>P26</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O28" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="O28" s="10">
         <f>P27</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P28" s="32" t="e">
+        <v>0</v>
+      </c>
+      <c r="P28" s="32">
         <f>$O$24*L16-$K$18/3</f>
-        <v>#DIV/0!</v>
+        <v>4.9999956918986159</v>
       </c>
       <c r="S28">
         <f t="shared" si="1"/>
@@ -5632,14 +5632,14 @@
       </c>
       <c r="K30">
         <f>(J26+K27+L28)/3</f>
-        <v>10.722534602547794</v>
+        <v>10.722534602547791</v>
       </c>
       <c r="N30" t="s">
         <v>10</v>
       </c>
-      <c r="O30" t="e">
+      <c r="O30">
         <f>(N26+O27+P28)/3</f>
-        <v>#DIV/0!</v>
+        <v>5.099733333333333</v>
       </c>
       <c r="S30">
         <f t="shared" si="1"/>
@@ -5679,27 +5679,27 @@
     <row r="33" spans="10:20" x14ac:dyDescent="0.25">
       <c r="J33">
         <f>J26-K30</f>
-        <v>0</v>
+        <v>1.1994666666666696</v>
       </c>
       <c r="K33">
         <f>K26</f>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="L33">
         <f>L26</f>
         <v>0</v>
       </c>
-      <c r="N33" t="e">
+      <c r="N33">
         <f>N26-O30</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O33" t="e">
+        <v>1.1995184790731503</v>
+      </c>
+      <c r="O33">
         <f>O26</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P33" t="e">
+        <v>-2.0000863924074319</v>
+      </c>
+      <c r="P33">
         <f>P26</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="S33">
         <f t="shared" si="1"/>
@@ -5713,27 +5713,27 @@
     <row r="34" spans="10:20" x14ac:dyDescent="0.25">
       <c r="J34">
         <f>J27</f>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="K34">
         <f>K27-K30</f>
-        <v>0</v>
+        <v>-1.0997333333333312</v>
       </c>
       <c r="L34">
         <f>L27</f>
         <v>0</v>
       </c>
-      <c r="N34" t="e">
+      <c r="N34">
         <f>N27</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O34" t="e">
+        <v>-2.0000863924074319</v>
+      </c>
+      <c r="O34">
         <f>O27-O30</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P34" t="e">
+        <v>-1.0997808376384328</v>
+      </c>
+      <c r="P34">
         <f>P27</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="S34">
         <f t="shared" si="1"/>
@@ -5755,19 +5755,19 @@
       </c>
       <c r="L35">
         <f>L28-K30</f>
+        <v>-9.9733333333331231E-2</v>
+      </c>
+      <c r="N35">
+        <f>N28</f>
         <v>0</v>
       </c>
-      <c r="N35" t="e">
-        <f>N28</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O35" t="e">
+      <c r="O35">
         <f>O28</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P35" t="e">
+        <v>0</v>
+      </c>
+      <c r="P35">
         <f>P28-O30</f>
-        <v>#DIV/0!</v>
+        <v>-9.9737641434717084E-2</v>
       </c>
       <c r="S35">
         <f t="shared" si="1"/>
@@ -5794,14 +5794,14 @@
       </c>
       <c r="K37">
         <f>-(J26+K27+L28)</f>
-        <v>-32.167603807643381</v>
+        <v>-32.167603807643374</v>
       </c>
       <c r="N37" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="O37" t="e">
+      <c r="O37">
         <f>-(N26+O27+P28)</f>
-        <v>#DIV/0!</v>
+        <v>-15.299199999999999</v>
       </c>
       <c r="S37">
         <f t="shared" si="1"/>
@@ -5818,14 +5818,14 @@
       </c>
       <c r="K38" s="3">
         <f>SQRT(0.5*SUMPRODUCT(J33:L35,J33:L35))</f>
-        <v>0</v>
+        <v>2.3084714018876937</v>
       </c>
       <c r="N38" t="s">
         <v>19</v>
       </c>
-      <c r="O38" s="3" t="e">
+      <c r="O38" s="3">
         <f>SQRT(0.5*SUMPRODUCT(N33:P35,N33:P35))</f>
-        <v>#DIV/0!</v>
+        <v>2.3085711190886422</v>
       </c>
       <c r="S38">
         <f t="shared" si="1"/>
@@ -5852,14 +5852,14 @@
       </c>
       <c r="K40" s="7">
         <f>K38-$N$1*K37-$N$2</f>
-        <v>0</v>
+        <v>2.3084714018876928</v>
       </c>
       <c r="N40" t="s">
         <v>20</v>
       </c>
-      <c r="O40" s="7" t="e">
+      <c r="O40" s="7">
         <f>O38-$N$1*O37-$N$2</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="S40">
         <f t="shared" si="1"/>
@@ -5891,9 +5891,9 @@
       <c r="N42" t="s">
         <v>24</v>
       </c>
-      <c r="O42" t="e">
+      <c r="O42">
         <f>IF(O37*$N$1+$N$2&lt;$O$38,1,0)</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="S42">
         <f t="shared" si="1"/>

</xml_diff>